<commit_message>
pushed day 12 stuff
</commit_message>
<xml_diff>
--- a/Excel Task Sheet/DlitheInternshipDailyUpdates.xlsx
+++ b/Excel Task Sheet/DlitheInternshipDailyUpdates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajw\Documents\Dlithe Internship\Excel Task Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B2AB6C-00FC-42C9-A7A8-1432B352F509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFE2058-C056-421E-9936-7AF7F4404ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{404EA253-EA28-4425-AB59-CAADAF4B36E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Finding conversion of fehrenit to celcious,prime or not,operators ,conversion of binary to decimal and decimal to binary</t>
+  </si>
+  <si>
+    <t>Create a netflix like clone application with team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered Database concepts, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types of DB , NoSql,Cloud DB , In memory DB,ER relationships </t>
   </si>
 </sst>
 </file>
@@ -525,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21B87A4-F670-4738-AE14-783FB4ECCEC2}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -736,6 +745,25 @@
         <v>34</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45727</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45728</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="https://github.com/PrajwalPai21/Dlithe2/commit/e83f5848be8b9149804ef8616dae37cce7213502https://github.com/PrajwalPai21/Dlithe2/commit/3a7f4952d1634f6413ee58b64f33fc103ffecdd2" xr:uid="{1BD1D5D6-01A8-4644-A097-9EC79C9A646D}"/>

</xml_diff>

<commit_message>
Final Project Frontend and Backend
</commit_message>
<xml_diff>
--- a/Excel Task Sheet/DlitheInternshipDailyUpdates.xlsx
+++ b/Excel Task Sheet/DlitheInternshipDailyUpdates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajw\Documents\Dlithe Internship\Excel Task Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFE2058-C056-421E-9936-7AF7F4404ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AD84CE-3276-476D-9AA6-D65F0A4E1097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{404EA253-EA28-4425-AB59-CAADAF4B36E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -155,13 +155,85 @@
   </si>
   <si>
     <t xml:space="preserve">Types of DB , NoSql,Cloud DB , In memory DB,ER relationships </t>
+  </si>
+  <si>
+    <t>Relational Database</t>
+  </si>
+  <si>
+    <t>Discussed RDBMS concepts.</t>
+  </si>
+  <si>
+    <t>Project Work</t>
+  </si>
+  <si>
+    <t>Worked on DBMS topics and created applications.</t>
+  </si>
+  <si>
+    <t>Installation</t>
+  </si>
+  <si>
+    <t>Installed MySQL and discussed MYSql topics</t>
+  </si>
+  <si>
+    <t>Demonstration</t>
+  </si>
+  <si>
+    <t>Demonstrated the Movie project.</t>
+  </si>
+  <si>
+    <t>UML Diagram</t>
+  </si>
+  <si>
+    <t>Created tables and UML diagrams.</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Performed table creation and data insertion.</t>
+  </si>
+  <si>
+    <t>Query Operations</t>
+  </si>
+  <si>
+    <t>Performed fetching operations for various problem statements.</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Learned the basics of Java.</t>
+  </si>
+  <si>
+    <t>Java Features</t>
+  </si>
+  <si>
+    <t>Learned abstraction, polymorphism, etc.</t>
+  </si>
+  <si>
+    <t>Operators</t>
+  </si>
+  <si>
+    <t>Discussed logical and numerical operators.</t>
+  </si>
+  <si>
+    <t>Java Operations</t>
+  </si>
+  <si>
+    <t>Explored Java operations.</t>
+  </si>
+  <si>
+    <t>Use Cases</t>
+  </si>
+  <si>
+    <t>Discussed use cases and operations.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +254,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -205,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -216,8 +295,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -534,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21B87A4-F670-4738-AE14-783FB4ECCEC2}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -584,7 +679,7 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -763,6 +858,147 @@
       <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45729</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45730</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>45733</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>45734</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>45735</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>45736</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>45737</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>45740</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>45741</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>45742</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45743</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>45744</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>45748</v>
+      </c>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>